<commit_message>
feat: finish financial task
</commit_message>
<xml_diff>
--- a/results/contrastive/evaluation_results_google-bert_bert-base-uncased.xlsx
+++ b/results/contrastive/evaluation_results_google-bert_bert-base-uncased.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8515463917525773</v>
+        <v>0.831958762886598</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8524319163260782</v>
+        <v>0.8330869608491775</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8515463917525773</v>
+        <v>0.831958762886598</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8546236742566817</v>
+        <v>0.8364940290651653</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7370496545967165</v>
+        <v>0.7039220174718617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>